<commit_message>
Financial Values imported from excel
</commit_message>
<xml_diff>
--- a/Financial Values.xlsx
+++ b/Financial Values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Objective</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>lt</t>
+  </si>
+  <si>
+    <t>Risky</t>
+  </si>
+  <si>
+    <t>Revenue Growth</t>
+  </si>
+  <si>
+    <t>revenuegrowth</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>beta</t>
   </si>
 </sst>
 </file>
@@ -395,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,20 +485,74 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
         <v>2000000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Url generation implements Standard and between logic. Next to incorporate view and order_by logic
</commit_message>
<xml_diff>
--- a/Financial Values.xlsx
+++ b/Financial Values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Objective</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>gt</t>
-  </si>
-  <si>
     <t>Trailing Dividend Yield</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>Debt to Equity</t>
   </si>
   <si>
-    <t>debtoequity</t>
-  </si>
-  <si>
-    <t>lt</t>
-  </si>
-  <si>
     <t>Risky</t>
   </si>
   <si>
@@ -93,6 +84,21 @@
   </si>
   <si>
     <t>lower bound</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>~lt~</t>
+  </si>
+  <si>
+    <t>~gt~</t>
+  </si>
+  <si>
+    <t>debttoequity</t>
   </si>
 </sst>
 </file>
@@ -410,149 +416,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G2">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>1.1000000000000001</v>
       </c>
       <c r="G4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
         <v>2000000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
URL Builder is complete
</commit_message>
<xml_diff>
--- a/Financial Values.xlsx
+++ b/Financial Values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Objective</t>
   </si>
@@ -99,6 +99,36 @@
   </si>
   <si>
     <t>debttoequity</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>asc</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Price to Book</t>
+  </si>
+  <si>
+    <t>pricetobook</t>
+  </si>
+  <si>
+    <t>Price to Earnings</t>
+  </si>
+  <si>
+    <t>pricetoearnings</t>
+  </si>
+  <si>
+    <t>Price to Revenue</t>
+  </si>
+  <si>
+    <t>pricetorevenue</t>
+  </si>
+  <si>
+    <t>desc</t>
   </si>
 </sst>
 </file>
@@ -416,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,24 +595,120 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+    </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="F8">
+      <c r="F11">
         <v>2000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>